<commit_message>
Update UTIBE INYANG - TECHSAVIA EXCEL PROJECT.xlsx
</commit_message>
<xml_diff>
--- a/ASSIGNMENT/UTIBE INYANG - TECHSAVIA EXCEL PROJECT.xlsx
+++ b/ASSIGNMENT/UTIBE INYANG - TECHSAVIA EXCEL PROJECT.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\myTutorials\DataCamp\ASSIGNMENT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\portfolio\DataCamp\ASSIGNMENT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82E1F9A-9477-4E37-89EE-A6F35690795C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944E770B-F59E-43F7-83DF-9E251A5D1FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AE457EBE-DAB4-4A63-BF59-D8445F378BE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="877" xr2:uid="{AE457EBE-DAB4-4A63-BF59-D8445F378BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Page001 (2)" sheetId="4" r:id="rId1"/>
-    <sheet name="1. Over 10 Years" sheetId="5" r:id="rId2"/>
-    <sheet name="2. Average Years of Experience" sheetId="6" r:id="rId3"/>
-    <sheet name="3. Average Salary Per Departmen" sheetId="7" r:id="rId4"/>
+    <sheet name="Relationship" sheetId="8" r:id="rId2"/>
+    <sheet name="1. Over 10 Years" sheetId="5" r:id="rId3"/>
+    <sheet name="2. Average Years of Experience" sheetId="6" r:id="rId4"/>
+    <sheet name="3. Average Salary Per Departmen" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="YearsExperience">'Page001 (2)'!$G:$G</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="134">
   <si>
     <t>EmpID</t>
   </si>
@@ -430,10 +431,31 @@
     <t>Average of Salary</t>
   </si>
   <si>
-    <t>p</t>
-  </si>
-  <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Average Salary</t>
+  </si>
+  <si>
+    <t>Employee Class</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Exployees By Country</t>
+  </si>
+  <si>
+    <t>Exployees By City</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Total Employees</t>
+  </si>
+  <si>
+    <t>Count of Department</t>
   </si>
 </sst>
 </file>
@@ -443,7 +465,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +480,18 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -554,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -582,11 +616,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -630,6 +686,1104 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Page001 (2)'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>YearsExperience</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Page001 (2)'!$F$2:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>78960.73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105887.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97023.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>115450.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>98400.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76500.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>134200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>112300.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89400.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68500.899999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60200.45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>121300.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99800.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>109500.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>71500.55</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85000.65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>125700.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>88000.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>104500.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>78200.350000000006</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>69800.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>134800.95000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>58200.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>93600.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>128300.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>74500.350000000006</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>81000.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Page001 (2)'!$G$2:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-383A-41AB-87E1-CA88A9103120}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="545308496"/>
+        <c:axId val="545325296"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="545308496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="545325296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="545325296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="545308496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4F71DF4-3103-6EB0-191A-0059C62F2816}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="utibe bassey" refreshedDate="45941.082527199076" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{CBCCBDAA-2829-4458-9C2C-8742399ECD25}">
   <cacheSource type="worksheet">
@@ -665,7 +1819,14 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.3" maxValue="15"/>
     </cacheField>
     <cacheField name="Country" numFmtId="49">
-      <sharedItems/>
+      <sharedItems count="6">
+        <s v="Canada"/>
+        <s v="UK"/>
+        <s v="USA"/>
+        <s v="India"/>
+        <s v="France"/>
+        <s v="Germany"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="City" numFmtId="49">
       <sharedItems/>
@@ -689,7 +1850,7 @@
     <d v="2012-02-14T00:00:00"/>
     <n v="78960.73"/>
     <n v="13.1"/>
-    <s v="Canada"/>
+    <x v="0"/>
     <s v="Toronto"/>
   </r>
   <r>
@@ -700,7 +1861,7 @@
     <d v="2018-10-07T00:00:00"/>
     <n v="105887.97"/>
     <n v="14.8"/>
-    <s v="UK"/>
+    <x v="1"/>
     <s v="Berlin"/>
   </r>
   <r>
@@ -711,7 +1872,7 @@
     <d v="2019-10-24T00:00:00"/>
     <n v="97023.2"/>
     <n v="1.3"/>
-    <s v="Canada"/>
+    <x v="0"/>
     <s v="Berlin"/>
   </r>
   <r>
@@ -722,7 +1883,7 @@
     <d v="2016-06-01T00:00:00"/>
     <n v="125500"/>
     <n v="11.4"/>
-    <s v="USA"/>
+    <x v="2"/>
     <s v="New York"/>
   </r>
   <r>
@@ -733,7 +1894,7 @@
     <d v="2020-03-15T00:00:00"/>
     <n v="115450.5"/>
     <n v="4.5"/>
-    <s v="India"/>
+    <x v="3"/>
     <s v="Delhi"/>
   </r>
   <r>
@@ -744,7 +1905,7 @@
     <d v="2015-09-21T00:00:00"/>
     <n v="98400.75"/>
     <n v="9.6999999999999993"/>
-    <s v="Canada"/>
+    <x v="0"/>
     <s v="Toronto"/>
   </r>
   <r>
@@ -755,7 +1916,7 @@
     <d v="2017-12-11T00:00:00"/>
     <n v="76500.2"/>
     <n v="6.1"/>
-    <s v="France"/>
+    <x v="4"/>
     <s v="Paris"/>
   </r>
   <r>
@@ -766,7 +1927,7 @@
     <d v="2014-07-25T00:00:00"/>
     <n v="134200"/>
     <n v="12"/>
-    <s v="USA"/>
+    <x v="2"/>
     <s v="Chicago"/>
   </r>
   <r>
@@ -777,7 +1938,7 @@
     <d v="2019-01-09T00:00:00"/>
     <n v="112300.65"/>
     <n v="3.9"/>
-    <s v="Germany"/>
+    <x v="5"/>
     <s v="Berlin"/>
   </r>
   <r>
@@ -788,7 +1949,7 @@
     <d v="2013-05-30T00:00:00"/>
     <n v="89400.8"/>
     <n v="14.2"/>
-    <s v="Canada"/>
+    <x v="0"/>
     <s v="Montreal"/>
   </r>
   <r>
@@ -799,7 +1960,7 @@
     <d v="2018-02-17T00:00:00"/>
     <n v="68500.899999999994"/>
     <n v="5.7"/>
-    <s v="USA"/>
+    <x v="2"/>
     <s v="Boston"/>
   </r>
   <r>
@@ -810,7 +1971,7 @@
     <d v="2021-06-20T00:00:00"/>
     <n v="60200.45"/>
     <n v="2.1"/>
-    <s v="France"/>
+    <x v="4"/>
     <s v="Lyon"/>
   </r>
   <r>
@@ -821,7 +1982,7 @@
     <d v="2016-08-05T00:00:00"/>
     <n v="121300.1"/>
     <n v="8.5"/>
-    <s v="India"/>
+    <x v="3"/>
     <s v="Mumbai"/>
   </r>
   <r>
@@ -832,7 +1993,7 @@
     <d v="2017-10-19T00:00:00"/>
     <n v="99800.75"/>
     <n v="7.3"/>
-    <s v="Canada"/>
+    <x v="0"/>
     <s v="Vancouver"/>
   </r>
   <r>
@@ -843,7 +2004,7 @@
     <d v="2014-11-25T00:00:00"/>
     <n v="109500.25"/>
     <n v="10.199999999999999"/>
-    <s v="UK"/>
+    <x v="1"/>
     <s v="London"/>
   </r>
   <r>
@@ -854,7 +2015,7 @@
     <d v="2019-04-14T00:00:00"/>
     <n v="71500.55"/>
     <n v="4"/>
-    <s v="USA"/>
+    <x v="2"/>
     <s v="Miami"/>
   </r>
   <r>
@@ -865,7 +2026,7 @@
     <d v="2015-01-09T00:00:00"/>
     <n v="85000.65"/>
     <n v="9.5"/>
-    <s v="France"/>
+    <x v="4"/>
     <s v="Paris"/>
   </r>
   <r>
@@ -876,7 +2037,7 @@
     <d v="2022-07-13T00:00:00"/>
     <n v="125700.85"/>
     <n v="2.5"/>
-    <s v="India"/>
+    <x v="3"/>
     <s v="Bangalore"/>
   </r>
   <r>
@@ -887,7 +2048,7 @@
     <d v="2013-03-18T00:00:00"/>
     <n v="88000.4"/>
     <n v="15"/>
-    <s v="Canada"/>
+    <x v="0"/>
     <s v="Toronto"/>
   </r>
   <r>
@@ -898,7 +2059,7 @@
     <d v="2020-08-29T00:00:00"/>
     <n v="104500.7"/>
     <n v="3.3"/>
-    <s v="UK"/>
+    <x v="1"/>
     <s v="Manchester"/>
   </r>
   <r>
@@ -909,7 +2070,7 @@
     <d v="2016-12-02T00:00:00"/>
     <n v="78200.350000000006"/>
     <n v="6.9"/>
-    <s v="USA"/>
+    <x v="2"/>
     <s v="Chicago"/>
   </r>
   <r>
@@ -920,7 +2081,7 @@
     <d v="2018-09-17T00:00:00"/>
     <n v="69800.25"/>
     <n v="5.2"/>
-    <s v="Germany"/>
+    <x v="5"/>
     <s v="Hamburg"/>
   </r>
   <r>
@@ -931,7 +2092,7 @@
     <d v="2012-04-22T00:00:00"/>
     <n v="134800.95000000001"/>
     <n v="14.6"/>
-    <s v="USA"/>
+    <x v="2"/>
     <s v="San Francisco"/>
   </r>
   <r>
@@ -942,7 +2103,7 @@
     <d v="2019-07-03T00:00:00"/>
     <n v="58200.800000000003"/>
     <n v="3.1"/>
-    <s v="UK"/>
+    <x v="1"/>
     <s v="Bristol"/>
   </r>
   <r>
@@ -953,7 +2114,7 @@
     <d v="2017-05-30T00:00:00"/>
     <n v="93600.6"/>
     <n v="7.7"/>
-    <s v="India"/>
+    <x v="3"/>
     <s v="Hyderabad"/>
   </r>
   <r>
@@ -964,7 +2125,7 @@
     <d v="2014-10-27T00:00:00"/>
     <n v="128300.2"/>
     <n v="11.1"/>
-    <s v="France"/>
+    <x v="4"/>
     <s v="Paris"/>
   </r>
   <r>
@@ -975,7 +2136,7 @@
     <d v="2016-01-11T00:00:00"/>
     <n v="74500.350000000006"/>
     <n v="8.1999999999999993"/>
-    <s v="Canada"/>
+    <x v="0"/>
     <s v="Ottawa"/>
   </r>
   <r>
@@ -986,14 +2147,115 @@
     <d v="2015-07-19T00:00:00"/>
     <n v="81000.55"/>
     <n v="9.9"/>
-    <s v="USA"/>
+    <x v="2"/>
     <s v="Atlanta"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9405A1C4-34E5-4FBC-A76E-1CF0B119EBF5}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{290816FB-E4AD-4074-9879-5B6C8A579DCA}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:H11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Department" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9405A1C4-34E5-4FBC-A76E-1CF0B119EBF5}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1069,8 +2331,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85ABC0BC-63E6-43B1-9DD6-CC9AE0A71CBB}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85ABC0BC-63E6-43B1-9DD6-CC9AE0A71CBB}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1138,22 +2400,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BB4A1725-3A41-4D61-8F79-AC7B98453417}" name="Table4" displayName="Table4" ref="A1:K29" totalsRowShown="0">
-  <autoFilter ref="A1:K29" xr:uid="{BB4A1725-3A41-4D61-8F79-AC7B98453417}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{9F12543F-2710-4EBD-8933-D6D44EECAAE8}" name="EmpID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B4C398C0-1840-473E-9C01-FEFAA8113C27}" name="FullName" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{D68B742F-EF15-4887-944E-D0AD23EE9F53}" name="JobTitle" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{F777E252-56F2-4689-952F-918224570F14}" name="Department" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{195DD26D-0479-46A7-825D-BE33FB2D5155}" name="HireDate" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4BA3FA23-4B5B-402D-8D4E-AD213AA77FE6}" name="Salary" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{9802B74F-3CF5-4E2D-9B71-0D63D11CB032}" name="YearsExperience" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{9B276F49-10FE-4D13-A4E6-B3754298888D}" name="Country" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{EAF6119C-4263-4DA2-8BC5-612DCA10AF6E}" name="City" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{2DF77886-2237-463B-B8ED-18F1ABD272C4}" name="Employed Over 10 Years" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BB4A1725-3A41-4D61-8F79-AC7B98453417}" name="Table4" displayName="Table4" ref="A1:P29" totalsRowShown="0">
+  <autoFilter ref="A1:P29" xr:uid="{BB4A1725-3A41-4D61-8F79-AC7B98453417}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{9F12543F-2710-4EBD-8933-D6D44EECAAE8}" name="EmpID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{B4C398C0-1840-473E-9C01-FEFAA8113C27}" name="FullName" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{D68B742F-EF15-4887-944E-D0AD23EE9F53}" name="JobTitle" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{F777E252-56F2-4689-952F-918224570F14}" name="Department" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{195DD26D-0479-46A7-825D-BE33FB2D5155}" name="HireDate" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{4BA3FA23-4B5B-402D-8D4E-AD213AA77FE6}" name="Salary" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{9802B74F-3CF5-4E2D-9B71-0D63D11CB032}" name="YearsExperience" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{9B276F49-10FE-4D13-A4E6-B3754298888D}" name="Country" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{EAF6119C-4263-4DA2-8BC5-612DCA10AF6E}" name="City" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{2DF77886-2237-463B-B8ED-18F1ABD272C4}" name="Employed Over 10 Years" dataDxfId="6">
       <calculatedColumnFormula>IF(G2&gt;10, "Over 10 Years", "Less Than 10 Years")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D629F377-EC6A-4955-8550-7B0CEAFB2C28}" name="Column1"/>
+    <tableColumn id="11" xr3:uid="{C96CBD4A-96D8-4099-8050-C8EAB52D03CC}" name="Average Salary" dataDxfId="5">
+      <calculatedColumnFormula>AVERAGEIF($D:$D, D2, $F:$F)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{0C57332C-59E0-47DA-85EB-48C1F726C409}" name="Employee Class" dataDxfId="4">
+      <calculatedColumnFormula>IF(F2 &gt; K2, "High class", "Normal")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{5DA06ECF-C5AC-4D30-9133-016BB28A1B2C}" name="Exployees By Country" dataDxfId="3">
+      <calculatedColumnFormula>COUNTIF(H2:H29, H2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{1BDC1F86-DEFF-437D-902F-F604D208AC44}" name="Exployees By City" dataDxfId="2">
+      <calculatedColumnFormula>COUNTIF(I2:I29, I2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{A60F0671-7C84-489E-9F6B-9770700503BD}" name="Column1" dataDxfId="1">
+      <calculatedColumnFormula>MAX(M2:M29)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{E0D6EC9F-A0D7-46DB-9AF6-9C5932BFFCBD}" name="Column2" dataDxfId="0">
+      <calculatedColumnFormula>INDEX(H2:H29, MATCH(MAX(M2:M29), M2:M29, 0))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1476,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D25EBA1-1F77-4654-9966-950FAEB7D0A2}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F1" activeCellId="1" sqref="G1:G1048576 F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,9 +2773,13 @@
     <col min="8" max="8" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1530,8 +2813,23 @@
       <c r="K1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O1" t="s">
+        <v>125</v>
+      </c>
+      <c r="P1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1563,8 +2861,32 @@
         <f>IF(G2&gt;10, "Over 10 Years", "Less Than 10 Years")</f>
         <v>Over 10 Years</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <f>AVERAGEIF($D:$D, D2, $F:$F)</f>
+        <v>91752.645999999993</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L29" si="0">IF(F2 &gt; K2, "High class", "Normal")</f>
+        <v>Normal</v>
+      </c>
+      <c r="M2" s="25">
+        <f>COUNTIF(H2:H29, H2)</f>
+        <v>7</v>
+      </c>
+      <c r="N2" s="25">
+        <f>COUNTIF(I2:I29, I2)</f>
+        <v>3</v>
+      </c>
+      <c r="O2" s="25">
+        <f t="shared" ref="O2:O29" si="1">MAX(M2:M29)</f>
+        <v>7</v>
+      </c>
+      <c r="P2" s="26" t="str">
+        <f t="shared" ref="P2:P29" si="2">INDEX(H2:H29, MATCH(MAX(M2:M29), M2:M29, 0))</f>
+        <v>Canada</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1593,11 +2915,35 @@
         <v>20</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J29" si="0">IF(G3&gt;10, "Over 10 Years", "Less Than 10 Years")</f>
+        <f t="shared" ref="J3:J29" si="3">IF(G3&gt;10, "Over 10 Years", "Less Than 10 Years")</f>
         <v>Over 10 Years</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <f t="shared" ref="K3:K29" si="4">AVERAGEIF($D:$D, D3, $F:$F)</f>
+        <v>112980.15249999998</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>Normal</v>
+      </c>
+      <c r="M3" s="25">
+        <f t="shared" ref="M3:M29" si="5">COUNTIF(H3:H30, H3)</f>
+        <v>4</v>
+      </c>
+      <c r="N3" s="25">
+        <f>COUNTIF(I3:I30, I3)</f>
+        <v>3</v>
+      </c>
+      <c r="O3" s="25">
+        <f>MAX(M3:M30)</f>
+        <v>7</v>
+      </c>
+      <c r="P3" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1626,11 +2972,35 @@
         <v>20</v>
       </c>
       <c r="J4" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>90305.05</v>
+      </c>
+      <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M4" s="25">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N4" s="25">
+        <f>COUNTIF(I4:I31, I4)</f>
+        <v>2</v>
+      </c>
+      <c r="O4" s="25">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P4" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1659,11 +3029,35 @@
         <v>30</v>
       </c>
       <c r="J5" t="str">
+        <f t="shared" si="3"/>
+        <v>Over 10 Years</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>130150.47500000001</v>
+      </c>
+      <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>Over 10 Years</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M5" s="25">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="N5" s="25">
+        <f>COUNTIF(I5:I32, I5)</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="25">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P5" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1692,11 +3086,35 @@
         <v>35</v>
       </c>
       <c r="J6" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>112980.15249999998</v>
+      </c>
+      <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M6" s="25">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N6" s="25">
+        <f>COUNTIF(I6:I33, I6)</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="P6" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1725,11 +3143,35 @@
         <v>14</v>
       </c>
       <c r="J7" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>91752.645999999993</v>
+      </c>
+      <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M7" s="25">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="N7" s="25">
+        <f>COUNTIF(I7:I34, I7)</f>
+        <v>2</v>
+      </c>
+      <c r="O7" s="25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="P7" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1758,11 +3200,35 @@
         <v>44</v>
       </c>
       <c r="J8" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>72875.387499999997</v>
+      </c>
+      <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M8" s="25">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N8" s="25">
+        <f>COUNTIF(I8:I35, I8)</f>
+        <v>3</v>
+      </c>
+      <c r="O8" s="25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="P8" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1791,11 +3257,35 @@
         <v>48</v>
       </c>
       <c r="J9" t="str">
+        <f t="shared" si="3"/>
+        <v>Over 10 Years</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>112980.15249999998</v>
+      </c>
+      <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>Over 10 Years</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M9" s="25">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N9" s="25">
+        <f>COUNTIF(I9:I36, I9)</f>
+        <v>2</v>
+      </c>
+      <c r="O9" s="25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="P9" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1824,14 +3314,35 @@
         <v>20</v>
       </c>
       <c r="J10" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>90305.05</v>
+      </c>
+      <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-      <c r="K10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M10" s="25">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N10" s="25">
+        <f>COUNTIF(I10:I37, I10)</f>
+        <v>1</v>
+      </c>
+      <c r="O10" s="25">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="P10" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1860,11 +3371,35 @@
         <v>57</v>
       </c>
       <c r="J11" t="str">
+        <f t="shared" si="3"/>
+        <v>Over 10 Years</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>80025.5625</v>
+      </c>
+      <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>Over 10 Years</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M11" s="25">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N11" s="25">
+        <f>COUNTIF(I11:I38, I11)</f>
+        <v>1</v>
+      </c>
+      <c r="O11" s="25">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="P11" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -1893,11 +3428,35 @@
         <v>61</v>
       </c>
       <c r="J12" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>112980.15249999998</v>
+      </c>
+      <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M12" s="25">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="N12" s="25">
+        <f>COUNTIF(I12:I39, I12)</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="25">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="P12" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1926,11 +3485,35 @@
         <v>65</v>
       </c>
       <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>72875.387499999997</v>
+      </c>
+      <c r="L13" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M13" s="25">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N13" s="25">
+        <f>COUNTIF(I13:I40, I13)</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="P13" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -1959,11 +3542,35 @@
         <v>69</v>
       </c>
       <c r="J14" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>112980.15249999998</v>
+      </c>
+      <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M14" s="25">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N14" s="25">
+        <f>COUNTIF(I14:I41, I14)</f>
+        <v>1</v>
+      </c>
+      <c r="O14" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="P14" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -1992,11 +3599,35 @@
         <v>72</v>
       </c>
       <c r="J15" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>91752.645999999993</v>
+      </c>
+      <c r="L15" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M15" s="25">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N15" s="25">
+        <f>COUNTIF(I15:I42, I15)</f>
+        <v>1</v>
+      </c>
+      <c r="O15" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="P15" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2025,11 +3656,35 @@
         <v>75</v>
       </c>
       <c r="J16" t="str">
+        <f t="shared" si="3"/>
+        <v>Over 10 Years</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>90305.05</v>
+      </c>
+      <c r="L16" t="str">
         <f t="shared" si="0"/>
-        <v>Over 10 Years</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M16" s="25">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N16" s="25">
+        <f>COUNTIF(I16:I43, I16)</f>
+        <v>1</v>
+      </c>
+      <c r="O16" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="P16" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -2058,11 +3713,35 @@
         <v>79</v>
       </c>
       <c r="J17" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>80025.5625</v>
+      </c>
+      <c r="L17" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M17" s="25">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N17" s="25">
+        <f>COUNTIF(I17:I44, I17)</f>
+        <v>1</v>
+      </c>
+      <c r="O17" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="P17" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -2091,11 +3770,35 @@
         <v>44</v>
       </c>
       <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>72875.387499999997</v>
+      </c>
+      <c r="L18" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M18" s="25">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N18" s="25">
+        <f>COUNTIF(I18:I45, I18)</f>
+        <v>2</v>
+      </c>
+      <c r="O18" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="P18" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -2124,11 +3827,35 @@
         <v>85</v>
       </c>
       <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>112980.15249999998</v>
+      </c>
+      <c r="L19" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M19" s="25">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N19" s="25">
+        <f>COUNTIF(I19:I46, I19)</f>
+        <v>1</v>
+      </c>
+      <c r="O19" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="P19" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -2157,11 +3884,35 @@
         <v>14</v>
       </c>
       <c r="J20" t="str">
+        <f t="shared" si="3"/>
+        <v>Over 10 Years</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>91752.645999999993</v>
+      </c>
+      <c r="L20" t="str">
         <f t="shared" si="0"/>
-        <v>Over 10 Years</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M20" s="25">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N20" s="25">
+        <f>COUNTIF(I20:I47, I20)</f>
+        <v>1</v>
+      </c>
+      <c r="O20" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="P20" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -2190,11 +3941,35 @@
         <v>91</v>
       </c>
       <c r="J21" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>112980.15249999998</v>
+      </c>
+      <c r="L21" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M21" s="25">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N21" s="25">
+        <f>COUNTIF(I21:I48, I21)</f>
+        <v>1</v>
+      </c>
+      <c r="O21" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="P21" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -2223,11 +3998,35 @@
         <v>48</v>
       </c>
       <c r="J22" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>80025.5625</v>
+      </c>
+      <c r="L22" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M22" s="25">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N22" s="25">
+        <f>COUNTIF(I22:I49, I22)</f>
+        <v>1</v>
+      </c>
+      <c r="O22" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="P22" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -2256,11 +4055,35 @@
         <v>97</v>
       </c>
       <c r="J23" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>72875.387499999997</v>
+      </c>
+      <c r="L23" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M23" s="25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N23" s="25">
+        <f>COUNTIF(I23:I50, I23)</f>
+        <v>1</v>
+      </c>
+      <c r="O23" s="25">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="P23" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -2289,11 +4112,35 @@
         <v>101</v>
       </c>
       <c r="J24" t="str">
+        <f t="shared" si="3"/>
+        <v>Over 10 Years</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>130150.47500000001</v>
+      </c>
+      <c r="L24" t="str">
         <f t="shared" si="0"/>
-        <v>Over 10 Years</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M24" s="25">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="N24" s="25">
+        <f>COUNTIF(I24:I51, I24)</f>
+        <v>1</v>
+      </c>
+      <c r="O24" s="25">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="P24" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -2322,11 +4169,35 @@
         <v>105</v>
       </c>
       <c r="J25" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>90305.05</v>
+      </c>
+      <c r="L25" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M25" s="25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N25" s="25">
+        <f>COUNTIF(I25:I52, I25)</f>
+        <v>1</v>
+      </c>
+      <c r="O25" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P25" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>UK</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -2355,11 +4226,35 @@
         <v>108</v>
       </c>
       <c r="J26" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>91752.645999999993</v>
+      </c>
+      <c r="L26" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M26" s="25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N26" s="25">
+        <f>COUNTIF(I26:I53, I26)</f>
+        <v>1</v>
+      </c>
+      <c r="O26" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P26" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>India</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>109</v>
       </c>
@@ -2388,11 +4283,35 @@
         <v>44</v>
       </c>
       <c r="J27" t="str">
+        <f t="shared" si="3"/>
+        <v>Over 10 Years</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>112980.15249999998</v>
+      </c>
+      <c r="L27" t="str">
         <f t="shared" si="0"/>
-        <v>Over 10 Years</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>High class</v>
+      </c>
+      <c r="M27" s="25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N27" s="25">
+        <f>COUNTIF(I27:I54, I27)</f>
+        <v>1</v>
+      </c>
+      <c r="O27" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P27" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>France</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>112</v>
       </c>
@@ -2421,11 +4340,35 @@
         <v>115</v>
       </c>
       <c r="J28" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="4"/>
+        <v>90305.05</v>
+      </c>
+      <c r="L28" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Normal</v>
+      </c>
+      <c r="M28" s="25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N28" s="25">
+        <f>COUNTIF(I28:I55, I28)</f>
+        <v>1</v>
+      </c>
+      <c r="O28" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P28" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>Canada</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -2454,19 +4397,274 @@
         <v>119</v>
       </c>
       <c r="J29" t="str">
+        <f t="shared" si="3"/>
+        <v>Less Than 10 Years</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="4"/>
+        <v>80025.5625</v>
+      </c>
+      <c r="L29" t="str">
         <f t="shared" si="0"/>
-        <v>Less Than 10 Years</v>
+        <v>High class</v>
+      </c>
+      <c r="M29" s="25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N29" s="25">
+        <f>COUNTIF(I29:I56, I29)</f>
+        <v>1</v>
+      </c>
+      <c r="O29" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P29" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v>USA</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE56A81-5012-414A-B44C-6159C36FF204}">
+  <dimension ref="A3:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="25">
+        <v>4</v>
+      </c>
+      <c r="C5" s="25">
+        <v>1</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25">
+        <v>2</v>
+      </c>
+      <c r="H5" s="25">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <f>SUM(B5:H5)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25">
+        <v>3</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I11" si="0">SUM(B6:H6)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25">
+        <v>1</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25">
+        <v>1</v>
+      </c>
+      <c r="H7" s="25">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="25">
+        <v>1</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25">
+        <v>3</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25">
+        <v>2</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25">
+        <v>2</v>
+      </c>
+      <c r="H9" s="25">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25">
+        <v>3</v>
+      </c>
+      <c r="D10" s="25">
+        <v>2</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25">
+        <v>2</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="25">
+        <v>5</v>
+      </c>
+      <c r="C11" s="25">
+        <v>4</v>
+      </c>
+      <c r="D11" s="25">
+        <v>8</v>
+      </c>
+      <c r="E11" s="25">
+        <v>4</v>
+      </c>
+      <c r="F11" s="25">
+        <v>2</v>
+      </c>
+      <c r="G11" s="25">
+        <v>5</v>
+      </c>
+      <c r="H11" s="25">
+        <v>28</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A36013-5A4A-406C-BF58-2AC3886F408F}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -2781,7 +4979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E3FFBC-53E8-41B0-B629-19AB276714EB}">
   <dimension ref="A3:B10"/>
   <sheetViews>
@@ -2864,7 +5062,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3AAE74-9F25-4E7B-BABE-384D9685A665}">
   <dimension ref="A3:B10"/>
   <sheetViews>

</xml_diff>